<commit_message>
update to final data release files
</commit_message>
<xml_diff>
--- a/data/Farmington_PFAS_FWstudy_Datarelease_README.xlsx
+++ b/data/Farmington_PFAS_FWstudy_Datarelease_README.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeb19004/Library/CloudStorage/GoogleDrive-brandtcontaminantslab@gmail.com/My Drive/Writing/Papers/PFAS/Farmington PFAS/FarmingtonPFAS_Food Web/Data files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeb19004/Library/CloudStorage/GoogleDrive-brandtcontaminantslab@gmail.com/My Drive/Writing/Papers/PFAS/Farmington PFAS/FarmingtonPFAS_Food Web/Data release/Submission files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EDA885-5A71-7E4A-B066-221D7AF6B14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7867CD-D7A0-DA4F-8A8D-A7F4323342C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34900" yWindow="500" windowWidth="26840" windowHeight="15940" xr2:uid="{B4F22606-AF3A-9744-A5A4-CD379D51AF94}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{B4F22606-AF3A-9744-A5A4-CD379D51AF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,10 +134,10 @@
     <t>Below reporting limit</t>
   </si>
   <si>
-    <t>Is the concentration below the reporting limit. Yes indicates the concentration is above the detection limit but below the reporting limit</t>
-  </si>
-  <si>
     <t>ND = not detected, NM = not measured, na = not available due to sample damage</t>
+  </si>
+  <si>
+    <t>Whether the concentration is below the reporting limit. Yes indicates the concentration is above the method detection limit, but below the reporting limit</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,7 +631,7 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>